<commit_message>
Added all anime in the short version of the flowchart
</commit_message>
<xml_diff>
--- a/src/anime-database.xlsx
+++ b/src/anime-database.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>Text</t>
   </si>
@@ -100,6 +100,66 @@
   </si>
   <si>
     <t>Don't overdo it</t>
+  </si>
+  <si>
+    <t>Want something typically Japanese?</t>
+  </si>
+  <si>
+    <t>Samurai are cool (even cooler with hip-hop music)</t>
+  </si>
+  <si>
+    <t>Samurai Champloo</t>
+  </si>
+  <si>
+    <t>I'VE HEARD THERE ARE SOME GIANT ROBOTS</t>
+  </si>
+  <si>
+    <t>TENGEN TOPPA GURREN LAGANN</t>
+  </si>
+  <si>
+    <t>I like the Ghibli movies, especially the spirit stuff</t>
+  </si>
+  <si>
+    <t>Mushishi</t>
+  </si>
+  <si>
+    <t>Something more Western, please</t>
+  </si>
+  <si>
+    <t>Fantasy action adventure?</t>
+  </si>
+  <si>
+    <t>Something gritty, edgy and with epic music</t>
+  </si>
+  <si>
+    <t>Attack on Titan</t>
+  </si>
+  <si>
+    <t>Arabian Nights road trip adventure, Avatar-style</t>
+  </si>
+  <si>
+    <t>Magi: The Labyrinth of Magic</t>
+  </si>
+  <si>
+    <t>Pirates of the Carribean meets Diablo</t>
+  </si>
+  <si>
+    <t>Shingeki no Bahamut: Genesis</t>
+  </si>
+  <si>
+    <t>I want more!</t>
+  </si>
+  <si>
+    <t>Extended version in development!</t>
+  </si>
+  <si>
+    <t>Psycho-Pass</t>
+  </si>
+  <si>
+    <t>Darker than Black</t>
+  </si>
+  <si>
+    <t>Steins;Gate</t>
   </si>
 </sst>
 </file>
@@ -444,10 +504,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,8 +515,8 @@
     <col min="1" max="1" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.5703125" style="2" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="4" max="4" width="8.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="23.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="13.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="27.7109375" style="2" customWidth="1"/>
   </cols>
@@ -513,7 +573,7 @@
         <v>9</v>
       </c>
       <c r="E3" s="1" t="str">
-        <f t="shared" ref="E3:E13" si="0">CONCATENATE("[",C3,"] ",D3)</f>
+        <f t="shared" ref="E3:E35" si="0">CONCATENATE("[",C3,"] ",D3)</f>
         <v>[2] Space western (Firefly, Guardians of the Galaxy)</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -633,6 +693,9 @@
         <f t="shared" si="0"/>
         <v>[1] Psychological police in a cyberpunk setting</v>
       </c>
+      <c r="G10" s="2" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="1">
@@ -645,6 +708,9 @@
         <f t="shared" si="0"/>
         <v>[2] Superpowers, X-Men style (Chinese Electric Batman)</v>
       </c>
+      <c r="G11" s="2" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="1">
@@ -657,6 +723,9 @@
         <f t="shared" si="0"/>
         <v>[3] Time travel experiment thriller</v>
       </c>
+      <c r="G12" s="2" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="1">
@@ -668,6 +737,225 @@
       <c r="E13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>[4] Don't overdo it</v>
+      </c>
+      <c r="F13" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[1] Samurai are cool (even cooler with hip-hop music)</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C15" s="1">
+        <v>2</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[2] I'VE HEARD THERE ARE SOME GIANT ROBOTS</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C16" s="1">
+        <v>3</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="E16" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[3] I like the Ghibli movies, especially the spirit stuff</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C17" s="1">
+        <v>4</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E17" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[4] Something more Western, please</v>
+      </c>
+      <c r="F17" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>4</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E18" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[1] Something gritty, edgy and with epic music</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C19" s="1">
+        <v>2</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[2] Arabian Nights road trip adventure, Avatar-style</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>3</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E20" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[3] Pirates of the Carribean meets Diablo</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="C21" s="1">
+        <v>4</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="E21" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>[4] I want more!</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E22" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E23" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E24" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E25" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E26" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E28" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E29" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E30" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E31" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
+      </c>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E35" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v xml:space="preserve">[] </v>
       </c>
     </row>
   </sheetData>

</xml_diff>